<commit_message>
updated kelsic files for colab
</commit_message>
<xml_diff>
--- a/colab/rounds_data/kelsic_Round2.xlsx
+++ b/colab/rounds_data/kelsic_Round2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,101 +458,111 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>4Q</t>
+          <t>4H</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.994</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>4V</t>
+          <t>4L</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.99775</v>
+        <v>0.9845</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>8M</t>
+          <t>4N</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.903</v>
+        <v>1.0115</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>14C</t>
+          <t>4Q</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9565</v>
+        <v>0.994</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>17M</t>
+          <t>4V</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.988</v>
+        <v>0.99775</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>32C</t>
+          <t>5M</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.97</v>
+        <v>1.038</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>62C</t>
+          <t>8C</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.962</v>
+        <v>0.8985</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>63C</t>
+          <t>8Q</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.833</v>
+        <v>0.913</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>68M</t>
+          <t>12C</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.964</v>
+        <v>0.7385</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>68T</t>
+          <t>12M</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.9565</v>
+        <v>1.012</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>71C</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>